<commit_message>
Updates for mapping test generation
</commit_message>
<xml_diff>
--- a/tests/data/scaffolding/v2/phenotype_HIVIND20_filled.xlsx
+++ b/tests/data/scaffolding/v2/phenotype_HIVIND20_filled.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmanko/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pmanko/code/who_l3_smart_tools/tests/data/scaffolding/v2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A8895F3B-92EC-6F47-A747-E8630596A945}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{213B5256-C1CD-F048-A3C3-D28740BA3542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="41120" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="880" windowWidth="41120" windowHeight="23780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="59">
+  <si>
+    <t>DAK ID</t>
+  </si>
   <si>
     <t>Short name</t>
   </si>
@@ -151,24 +154,6 @@
     <t>Phenotype Description</t>
   </si>
   <si>
-    <t>Gender</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Key population member type</t>
-  </si>
-  <si>
-    <t>TB diagnosis result</t>
-  </si>
-  <si>
-    <t>Presumptive TB</t>
-  </si>
-  <si>
-    <t>Testing entry point</t>
-  </si>
-  <si>
     <t>Counted as Numerator (0,1)</t>
   </si>
   <si>
@@ -197,9 +182,6 @@
   </si>
   <si>
     <t>Patient with negative HIV test in reporting period</t>
-  </si>
-  <si>
-    <t>Ω</t>
   </si>
   <si>
     <t>negative</t>
@@ -611,11 +593,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y14"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="L1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="M16" sqref="M16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -633,121 +615,121 @@
     <col min="17" max="19" width="50" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>53</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" ht="345" customHeight="1" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="345" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
@@ -768,76 +750,76 @@
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
     </row>
-    <row r="4" spans="1:25" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D4" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N4" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="O4" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>44</v>
-      </c>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="4"/>
+      <c r="O4" s="4"/>
+      <c r="P4" s="4"/>
+      <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
-      <c r="T4" s="4"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
-      <c r="Y4" s="4"/>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>40</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J5">
         <v>1</v>
@@ -845,104 +827,101 @@
       <c r="K5">
         <v>1</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-      <c r="M5" t="s">
-        <v>51</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>1</v>
-      </c>
-      <c r="Q5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>47</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
-      <c r="L6">
-        <v>1</v>
-      </c>
-      <c r="M6" t="s">
-        <v>54</v>
-      </c>
-      <c r="N6">
-        <v>0</v>
-      </c>
-      <c r="O6">
-        <v>0</v>
-      </c>
-      <c r="P6">
-        <v>0</v>
-      </c>
-      <c r="Q6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>49</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>46</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J7">
         <v>0</v>
       </c>
       <c r="K7">
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <v>0</v>
-      </c>
-      <c r="M7" t="s">
-        <v>51</v>
-      </c>
-      <c r="N7">
-        <v>0</v>
-      </c>
-      <c r="O7">
-        <v>0</v>
-      </c>
-      <c r="P7">
-        <v>0</v>
-      </c>
-      <c r="Q7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>58</v>
+        <v>52</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
       </c>
       <c r="I8">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J8">
         <v>0</v>
@@ -950,63 +929,66 @@
       <c r="K8">
         <v>0</v>
       </c>
-      <c r="L8">
-        <v>0</v>
-      </c>
-      <c r="N8">
-        <v>1</v>
-      </c>
-      <c r="O8">
-        <v>1</v>
-      </c>
-      <c r="P8">
-        <v>0</v>
-      </c>
-      <c r="Q8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J9">
         <v>0</v>
       </c>
       <c r="K9">
-        <v>1</v>
-      </c>
-      <c r="L9">
-        <v>1</v>
-      </c>
-      <c r="M9" t="s">
-        <v>51</v>
-      </c>
-      <c r="N9">
-        <v>0</v>
-      </c>
-      <c r="O9">
-        <v>0</v>
-      </c>
-      <c r="P9">
-        <v>0</v>
-      </c>
-      <c r="Q9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>6</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>46</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
       </c>
       <c r="I10">
         <v>1</v>
@@ -1015,68 +997,68 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10">
-        <v>0</v>
-      </c>
-      <c r="M10" t="s">
-        <v>51</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-      <c r="P10">
-        <v>0</v>
-      </c>
-      <c r="Q10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>61</v>
+        <v>55</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>46</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K11">
         <v>1</v>
       </c>
-      <c r="L11">
-        <v>0</v>
-      </c>
-      <c r="M11" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11">
-        <v>0</v>
-      </c>
-      <c r="O11">
-        <v>0</v>
-      </c>
-      <c r="P11">
-        <v>0</v>
-      </c>
-      <c r="Q11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>62</v>
+        <v>56</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>46</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
       </c>
       <c r="I12">
         <v>1</v>
@@ -1087,31 +1069,28 @@
       <c r="K12">
         <v>1</v>
       </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12" t="s">
-        <v>51</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
-      </c>
-      <c r="O12">
-        <v>1</v>
-      </c>
-      <c r="P12">
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>63</v>
+        <v>57</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
       </c>
       <c r="I13">
         <v>0</v>
@@ -1122,28 +1101,28 @@
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13">
-        <v>0</v>
-      </c>
-      <c r="N13">
-        <v>1</v>
-      </c>
-      <c r="O13">
-        <v>0</v>
-      </c>
-      <c r="P13">
-        <v>0</v>
-      </c>
-      <c r="Q13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>64</v>
+        <v>58</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
       </c>
       <c r="I14">
         <v>1</v>
@@ -1152,21 +1131,6 @@
         <v>1</v>
       </c>
       <c r="K14">
-        <v>0</v>
-      </c>
-      <c r="L14">
-        <v>0</v>
-      </c>
-      <c r="N14">
-        <v>1</v>
-      </c>
-      <c r="O14">
-        <v>1</v>
-      </c>
-      <c r="P14">
-        <v>1</v>
-      </c>
-      <c r="Q14">
         <v>1</v>
       </c>
     </row>

</xml_diff>